<commit_message>
liste produits et sous produits
</commit_message>
<xml_diff>
--- a/Classeur1.xlsx
+++ b/Classeur1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kurazul/Documents/Cours CESI/methodologie/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A662A367-D92E-9344-ADD8-3788D379171C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB54C682-D404-1947-A866-51D199B0FE73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{C94B01D0-8B92-F346-A296-24CA9E669CB1}"/>
+    <workbookView xWindow="43100" yWindow="-5920" windowWidth="28040" windowHeight="17440" xr2:uid="{C94B01D0-8B92-F346-A296-24CA9E669CB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Projet Méthodologie</t>
+  </si>
+  <si>
+    <t>Récuperer les données</t>
+  </si>
+  <si>
+    <t>Ttraiter les données</t>
+  </si>
+  <si>
+    <t>télécharger les données 1 fois par jours</t>
+  </si>
+  <si>
+    <t>afficher 1 ligne par match</t>
+  </si>
+  <si>
+    <t>récuperer l'ensemble des statitstiques possible d'un match</t>
+  </si>
+  <si>
+    <t>L'ensemble des matchs des divisions majeures</t>
+  </si>
+  <si>
+    <t>nombre de but mis par équipe</t>
+  </si>
+  <si>
+    <t>nombre de but encaissé par équipe</t>
+  </si>
+  <si>
+    <t>nombre de victoire</t>
+  </si>
+  <si>
+    <t>nombre de défaite</t>
+  </si>
+  <si>
+    <t>nombre de matche nul</t>
+  </si>
+  <si>
+    <t>nombre de but moyen par match</t>
+  </si>
+  <si>
+    <t>Afficher les données</t>
+  </si>
+  <si>
+    <t>dézipper les données</t>
+  </si>
+  <si>
+    <t>lire les fichiers des main leagues</t>
+  </si>
+  <si>
+    <t>Afficher les statistiques par main leagues</t>
+  </si>
+  <si>
+    <t>nombre de matches joués</t>
+  </si>
+  <si>
+    <t xml:space="preserve">etablir le classement de la saison </t>
+  </si>
+  <si>
+    <t>nombre de points</t>
+  </si>
+  <si>
+    <t>golaverage</t>
   </si>
 </sst>
 </file>
@@ -78,7 +138,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,23 +455,135 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFEE2B32-0C11-154A-B18F-FED9F438F5A5}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>